<commit_message>
Tabela agora gera coluna de inconsistencia \n *
</commit_message>
<xml_diff>
--- a/banco_de_dados/BD2.xlsx
+++ b/banco_de_dados/BD2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smart\Documents\AHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smart\Documents\AHP\banco_de_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,10 +25,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,7 +557,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>